<commit_message>
Speakers didn't work. No sound
</commit_message>
<xml_diff>
--- a/Whips-BOM.xlsx
+++ b/Whips-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spolsky/Library/CloudStorage/Dropbox/Arduino/Antenna2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6104144-2D03-E14A-A706-1B135FAAB86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBFC17A-4590-B747-AAC6-4711032BB8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14900" yWindow="9600" windowWidth="29880" windowHeight="15940" xr2:uid="{150F6CFE-C729-2E45-A4A5-336CC36D7694}"/>
+    <workbookView xWindow="20140" yWindow="9540" windowWidth="29880" windowHeight="15940" xr2:uid="{150F6CFE-C729-2E45-A4A5-336CC36D7694}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>Item</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>https://octopart.com/search?q=Traco+TSR1-2450E&amp;currency=USD&amp;specs=0</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
   <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -766,10 +769,10 @@
         <v>27</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G7">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>22</v>
@@ -825,16 +828,19 @@
         <v>31</v>
       </c>
       <c r="E10">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="I10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -848,11 +854,10 @@
         <v>27</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="G11">
-        <f>9+17</f>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>35</v>
@@ -872,8 +877,7 @@
         <v>39</v>
       </c>
       <c r="E12">
-        <f>27*4</f>
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>108</v>
@@ -883,6 +887,9 @@
       </c>
       <c r="H12" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -896,10 +903,10 @@
         <v>27</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>71</v>
@@ -920,10 +927,10 @@
         <v>54</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>44</v>

</xml_diff>